<commit_message>
Hemos añadido tareas y ejecutables varios
</commit_message>
<xml_diff>
--- a/Plantilla Tasksv2.xlsx
+++ b/Plantilla Tasksv2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY VAIO\Desktop\APP\ISO-Xcape\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{89F6F23C-B79C-4A08-A49E-FC6FD1ECE6F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12708" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="85">
   <si>
     <t>Story Title</t>
   </si>
@@ -99,9 +100,6 @@
     <t>Mostrar información introducida por pantalla</t>
   </si>
   <si>
-    <t>Crear BBDD</t>
-  </si>
-  <si>
     <t>Crear tabla</t>
   </si>
   <si>
@@ -136,13 +134,160 @@
   </si>
   <si>
     <t>45 min</t>
+  </si>
+  <si>
+    <t>X-4</t>
+  </si>
+  <si>
+    <t>Desarrollo modulo de contacto</t>
+  </si>
+  <si>
+    <t>Desarollar modulo de contacto, acerca de la compañía, otros viajes, etc. (telefónos, correos,fax)</t>
+  </si>
+  <si>
+    <t>Creación de BBDD</t>
+  </si>
+  <si>
+    <t>Creación de tablas correspondientes</t>
+  </si>
+  <si>
+    <t>X-X</t>
+  </si>
+  <si>
+    <t>Elección sistema de control de versiones</t>
+  </si>
+  <si>
+    <t>Instalación de Github</t>
+  </si>
+  <si>
+    <t>Creación Repositorio</t>
+  </si>
+  <si>
+    <t>Comprobación todo usuarios acceso GIT</t>
+  </si>
+  <si>
+    <t>Instalación MYSQL</t>
+  </si>
+  <si>
+    <t>Elección de entorno de desarrollo</t>
+  </si>
+  <si>
+    <t>Instalación de GayBeans</t>
+  </si>
+  <si>
+    <t>1 día</t>
+  </si>
+  <si>
+    <t>5 horas</t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <t>3 horas</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>35 min</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Se incluye familiarizarse con el entorno. Ninguno habia trabajado antes con github</t>
+  </si>
+  <si>
+    <t>Creado y borrad varias veces por cambios en los requisitos. Incluye repaso y aprendizaje de sql para aquellos que no han cursado BBDD</t>
+  </si>
+  <si>
+    <t>Conexión de Gaybeans con GIT</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos permite realizar commits directamente desde el propio entorno de programación </t>
+  </si>
+  <si>
+    <t>HECHO</t>
+  </si>
+  <si>
+    <t>Generación de querys correspondientes</t>
+  </si>
+  <si>
+    <t>Diseño/organización de carpetas del proyecto</t>
+  </si>
+  <si>
+    <t>Cordinación de los distintos modulos que tenemos hasta el momento</t>
+  </si>
+  <si>
+    <t>Comprobación de correcto funcionamiento</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>Comprobación de querys en CMD de MySQL</t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>problema con contraseñas de los distintos componentes del grupo (crear usuarios)</t>
+  </si>
+  <si>
+    <t>Incluye juntar códigos de los distintos miembros</t>
+  </si>
+  <si>
+    <t>Programación del código de dicho modulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hora </t>
+  </si>
+  <si>
+    <t>Conector a BBDD</t>
+  </si>
+  <si>
+    <t>1.5 horas</t>
+  </si>
+  <si>
+    <t>Alex &amp; Fernando</t>
+  </si>
+  <si>
+    <t>Incluye la creación de objetos, conectores, tratamiento de querys, ajustar la interfaz</t>
+  </si>
+  <si>
+    <t>Clonacíon de repositorio con Git-Bash</t>
+  </si>
+  <si>
+    <t>Instalación de Hyper-V</t>
+  </si>
+  <si>
+    <t>Instalación de máquina virtual</t>
+  </si>
+  <si>
+    <t>Comprobación de funcionamiento de APP mediante cmd</t>
+  </si>
+  <si>
+    <t>Creación de script</t>
+  </si>
+  <si>
+    <t>Problemas con contraseña y clonacion de repositorio</t>
+  </si>
+  <si>
+    <t>HECIHO</t>
+  </si>
+  <si>
+    <t>Creación Script Windows &amp; Linux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +297,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -224,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -256,6 +409,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,22 +728,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -610,7 +769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -634,7 +793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -646,31 +805,286 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43369</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43369</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6">
+        <v>43369</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A5:H6"/>
+    <mergeCell ref="A11:H12"/>
+    <mergeCell ref="A17:H18"/>
+    <mergeCell ref="A23:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -678,25 +1092,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H33" sqref="H32:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -722,397 +1136,605 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H16" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H17" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H21" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H22" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H28" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1122,43 +1744,131 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H29" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H30" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H31" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="B32" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>